<commit_message>
Finally fix past error of adding too large of a file in multiple commits
</commit_message>
<xml_diff>
--- a/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson11_ChiSquared.xlsx
+++ b/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson11_ChiSquared.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mountain" sheetId="1" r:id="rId1"/>
     <sheet name="cars" sheetId="3" r:id="rId2"/>
+    <sheet name="problem set" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
   <si>
     <t>n</t>
   </si>
@@ -113,6 +114,69 @@
   <si>
     <t>&lt;-- small effect</t>
   </si>
+  <si>
+    <t>dice</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>(goodness of fit b/c we have 1 nominal variable)</t>
+  </si>
+  <si>
+    <t>rolls</t>
+  </si>
+  <si>
+    <t>chi-crit</t>
+  </si>
+  <si>
+    <t>expected (fair die)</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>diff^2</t>
+  </si>
+  <si>
+    <t>diff^2/expected</t>
+  </si>
+  <si>
+    <t>&lt;- reject null = dice is biased</t>
+  </si>
+  <si>
+    <t>Titanic</t>
+  </si>
+  <si>
+    <t>survived?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Cabin</t>
+  </si>
+  <si>
+    <t>Steerage</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Accomodations -&gt; Is there a relationship between accomodations and survival rate?</t>
+  </si>
+  <si>
+    <t>&lt;-- can only choose  1 box + other 3 must automatically add up to the marginal totals</t>
+  </si>
+  <si>
+    <t>&lt;-- REJECT null the 2 variables are NOT independent = survival rate is correlated with/related to accomodations</t>
+  </si>
 </sst>
 </file>
 
@@ -121,7 +185,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +266,22 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -309,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -348,6 +428,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -381,9 +475,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -393,16 +484,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -427,13 +511,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>608864</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>56929</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -729,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD100"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:I7"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +840,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27">
+      <c r="B1" s="16">
         <v>100</v>
       </c>
       <c r="C1" s="2"/>
@@ -788,8 +872,8 @@
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="10"/>
@@ -816,11 +900,11 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="20"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="26"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -844,11 +928,11 @@
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="20"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -920,15 +1004,15 @@
       <c r="B7" s="1">
         <v>8.8900000000000007E-2</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="30"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -991,16 +1075,16 @@
       <c r="C10" s="3"/>
       <c r="D10" s="8"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="22"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="28"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="4"/>
       <c r="S10" s="2"/>
@@ -1045,12 +1129,12 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="25"/>
-      <c r="V12" s="25"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
     </row>
     <row r="13" spans="1:30" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
@@ -1058,8 +1142,8 @@
       <c r="C13" s="3"/>
       <c r="D13" s="8"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="9"/>
       <c r="I13" s="3"/>
       <c r="J13" s="2"/>
@@ -1069,20 +1153,20 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="25"/>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="25"/>
-      <c r="Z13" s="25"/>
-      <c r="AA13" s="25"/>
-      <c r="AB13" s="25"/>
-      <c r="AC13" s="25"/>
-      <c r="AD13" s="25"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+      <c r="V13" s="31"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="31"/>
+      <c r="Y13" s="31"/>
+      <c r="Z13" s="31"/>
+      <c r="AA13" s="31"/>
+      <c r="AB13" s="31"/>
+      <c r="AC13" s="31"/>
+      <c r="AD13" s="31"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
@@ -1325,10 +1409,10 @@
       <c r="T24" s="2"/>
     </row>
     <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="24"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -3015,10 +3099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="V31" sqref="V31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3031,380 +3115,767 @@
     <col min="8" max="8" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C2" s="1">
         <v>7</v>
       </c>
-      <c r="D16">
+      <c r="D2">
         <v>16</v>
       </c>
-      <c r="E16">
+      <c r="E2">
         <v>6</v>
       </c>
-      <c r="F16">
-        <f>SUM(C16:E16)</f>
+      <c r="F2">
+        <f>SUM(C2:E2)</f>
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C17">
+      <c r="C3">
         <v>43</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D3" s="13">
         <v>34</v>
       </c>
-      <c r="E17">
+      <c r="E3">
         <v>44</v>
       </c>
-      <c r="F17">
-        <f>SUM(C17:E17)</f>
+      <c r="F3">
+        <f>SUM(C3:E3)</f>
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="5"/>
-      <c r="C18">
-        <f>SUM(C16:C17)</f>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5"/>
+      <c r="C4">
+        <f>SUM(C2:C3)</f>
         <v>50</v>
       </c>
-      <c r="D18">
-        <f t="shared" ref="D18:E18" si="0">SUM(D16:D17)</f>
+      <c r="D4">
+        <f t="shared" ref="D4:E4" si="0">SUM(D2:D3)</f>
         <v>50</v>
       </c>
-      <c r="E18">
+      <c r="E4">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="F18">
-        <f>SUM(F16:F17)</f>
+      <c r="F4">
+        <f>SUM(F2:F3)</f>
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="33" t="s">
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="H8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" t="s">
+      <c r="I8" s="3"/>
+      <c r="J8" t="s">
         <v>11</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K8" t="s">
         <v>12</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="32">
-        <f>F23/COUNT(C16:E16)</f>
+      <c r="C9" s="18">
+        <f>F9/COUNT(C2:E2)</f>
         <v>9.6666666666666661</v>
       </c>
-      <c r="D23" s="32">
-        <f>C23</f>
+      <c r="D9" s="18">
+        <f>C9</f>
         <v>9.6666666666666661</v>
       </c>
-      <c r="E23" s="32">
-        <f>C23</f>
+      <c r="E9" s="18">
+        <f>C9</f>
         <v>9.6666666666666661</v>
       </c>
-      <c r="F23">
+      <c r="F9">
         <v>29</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J23" s="32">
-        <f>(C18*$F$16)/$F$18</f>
+      <c r="J9" s="18">
+        <f>(C4*$F$2)/$F$4</f>
         <v>9.6666666666666661</v>
       </c>
-      <c r="K23" s="32">
-        <f t="shared" ref="K23:L23" si="1">(D18*$F$16)/$F$18</f>
+      <c r="K9" s="18">
+        <f>(D4*$F$2)/$F$4</f>
         <v>9.6666666666666661</v>
       </c>
-      <c r="L23" s="32">
-        <f t="shared" si="1"/>
+      <c r="L9" s="18">
+        <f>(E4*$F$2)/$F$4</f>
         <v>9.6666666666666661</v>
       </c>
-      <c r="M23">
+      <c r="M9">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="5" t="s">
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="32">
-        <f>F24/COUNT(C17:E17)</f>
+      <c r="C10" s="18">
+        <f>F10/COUNT(C3:E3)</f>
         <v>40.333333333333336</v>
       </c>
-      <c r="D24" s="32">
-        <f>C24</f>
+      <c r="D10" s="18">
+        <f>C10</f>
         <v>40.333333333333336</v>
       </c>
-      <c r="E24" s="32">
-        <f>C24</f>
+      <c r="E10" s="18">
+        <f>C10</f>
         <v>40.333333333333336</v>
       </c>
-      <c r="F24">
+      <c r="F10">
         <v>121</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J24" s="32">
-        <f>(C18*$F$17)/$F$18</f>
+      <c r="J10" s="18">
+        <f>(C4*$F$3)/$F$4</f>
         <v>40.333333333333336</v>
       </c>
-      <c r="K24" s="32">
-        <f t="shared" ref="K24:L24" si="2">(D18*$F$17)/$F$18</f>
+      <c r="K10" s="18">
+        <f>(D4*$F$3)/$F$4</f>
         <v>40.333333333333336</v>
       </c>
-      <c r="L24" s="32">
-        <f t="shared" si="2"/>
+      <c r="L10" s="18">
+        <f>(E4*$F$3)/$F$4</f>
         <v>40.333333333333336</v>
       </c>
-      <c r="M24">
+      <c r="M10">
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="5"/>
-      <c r="C25">
-        <f>SUM(C23:C24)</f>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="5"/>
+      <c r="C11" s="37">
+        <f>SUM(C9:C10)</f>
         <v>50</v>
       </c>
-      <c r="D25">
-        <f t="shared" ref="D25" si="3">SUM(D23:D24)</f>
+      <c r="D11">
+        <f>SUM(D9:D10)</f>
         <v>50</v>
       </c>
-      <c r="E25">
-        <f t="shared" ref="E25" si="4">SUM(E23:E24)</f>
+      <c r="E11">
+        <f>SUM(E9:E10)</f>
         <v>50</v>
       </c>
-      <c r="F25">
+      <c r="F11">
         <v>150</v>
       </c>
-      <c r="I25" s="5"/>
-      <c r="J25">
-        <f>SUM(J23:J24)</f>
+      <c r="I11" s="5"/>
+      <c r="J11">
+        <f>SUM(J9:J10)</f>
         <v>50</v>
       </c>
-      <c r="K25">
-        <f t="shared" ref="K25" si="5">SUM(K23:K24)</f>
+      <c r="K11">
+        <f>SUM(K9:K10)</f>
         <v>50</v>
       </c>
-      <c r="L25">
-        <f t="shared" ref="L25" si="6">SUM(L23:L24)</f>
+      <c r="L11">
+        <f>SUM(L9:L10)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="1">
-        <f>SUM((C16-J23)^2/J23,(D16-K23)^2/K23,(E16-L23)^2/L23,(C17-J24)^2/J24,(D17-K24)^2/K24,(E17-L24)^2/L24)</f>
+      <c r="B13" s="1">
+        <f>SUM((C2-J9)^2/J9,(D2-K9)^2/K9,(E2-L9)^2/L9,(C3-J10)^2/J10,(D3-K10)^2/K10,(E3-L10)^2/L10)</f>
         <v>7.7799943003704781</v>
       </c>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="32">
-        <f>(COUNT(C23:E23)-1)*(COUNT(C23:C24)-1)</f>
+      <c r="B14" s="18">
+        <f>(COUNT(C9:E9)-1)*(COUNT(C9:C10)-1)</f>
         <v>2</v>
       </c>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="32">
+      <c r="B15" s="18">
         <v>5.9909999999999997</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="1">
-        <f>SQRT(B27/(F25*(COUNT(C23:C24)-1)))</f>
+      <c r="B16" s="1">
+        <f>SQRT(B13/(F11*(COUNT(C9:C10)-1)))</f>
         <v>0.22774246127838463</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="C37" s="1"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="C23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <f>B3-C3</f>
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f>D3^2</f>
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <f>E3/C3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D8" si="0">B4-C4</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E8" si="1">D4^2</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F8" si="2">E4/C4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1">
+        <f>SUM(B3:B8)</f>
+        <v>24</v>
+      </c>
+      <c r="C9" s="1">
+        <f>SUM(C3:C8)</f>
+        <v>24</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1">
+        <f>COUNT(A3:A8)-1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11.07</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1">
+        <f>SUM(F3:F8)</f>
+        <v>14.5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>299</v>
+      </c>
+      <c r="D18">
+        <v>186</v>
+      </c>
+      <c r="E18" s="1">
+        <f>SUM(C18:D18)</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>280</v>
+      </c>
+      <c r="D19">
+        <v>526</v>
+      </c>
+      <c r="E19" s="1">
+        <f>SUM(C19:D19)</f>
+        <v>806</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1">
+        <f>SUM(C18:C19)</f>
+        <v>579</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:E20" si="3">SUM(D18:D19)</f>
+        <v>712</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="3"/>
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="18">
+        <f>E23/2</f>
+        <v>242.5</v>
+      </c>
+      <c r="D23" s="18">
+        <f>C23</f>
+        <v>242.5</v>
+      </c>
+      <c r="E23">
+        <v>485</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" s="18">
+        <f>(C20*$E$18)/$E$20</f>
+        <v>217.51742835011618</v>
+      </c>
+      <c r="J23" s="18">
+        <f>(D20*$E$18)/$E$20</f>
+        <v>267.48257164988382</v>
+      </c>
+      <c r="K23" s="13">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="18">
+        <f>E24/2</f>
+        <v>403</v>
+      </c>
+      <c r="D24" s="18">
+        <f>C24</f>
+        <v>403</v>
+      </c>
+      <c r="E24">
+        <v>806</v>
+      </c>
+      <c r="G24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" s="18">
+        <f>(C20*$E$19)/$E$20</f>
+        <v>361.48257164988382</v>
+      </c>
+      <c r="J24" s="18">
+        <f>(D20*$E$19)/$E$20</f>
+        <v>444.51742835011618</v>
+      </c>
+      <c r="K24" s="13">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="37">
+        <f>SUM(C23:C24)</f>
+        <v>645.5</v>
+      </c>
+      <c r="D25">
+        <f>SUM(D23:D24)</f>
+        <v>645.5</v>
+      </c>
+      <c r="E25">
+        <v>1291</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="38">
+        <f>SUM(I23:I24)</f>
+        <v>579</v>
+      </c>
+      <c r="J25">
+        <f>SUM(J23:J24)</f>
+        <v>712</v>
+      </c>
+      <c r="K25" s="38">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1">
+        <v>3.8410000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1">
+        <f>SUM((C18-I23)^2/I23,(C19-I24)^2/I24,(D18-J23)^2/J23,(D19-J24)^2/J24)</f>
+        <v>88.648796387152103</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>